<commit_message>
feat: Implement backend API for dashboard
</commit_message>
<xml_diff>
--- a/server/expense_details.xlsx
+++ b/server/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,18 +416,51 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Groceries</v>
+        <v>food</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>4000</v>
       </c>
       <c r="C2" s="1">
+        <v>45881.250231481485</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Tuition fee</v>
+      </c>
+      <c r="B3">
+        <v>90000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45873.250231481485</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Travel</v>
+      </c>
+      <c r="B4">
+        <v>4000</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45872.250231481485</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Food</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="1">
         <v>45870.250231481485</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(budget): Implement budget creation and notification system
- Added full CRUD functionality for monthly budgets.
- Implemented real-time and session-based notifications for overspending.
- Designed an UI for displaying budget progress.
</commit_message>
<xml_diff>
--- a/server/expense_details.xlsx
+++ b/server/expense_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,62 +416,117 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>cat</v>
+        <v>fooD</v>
       </c>
       <c r="B2">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="C2" s="1">
-        <v>45883.250231481485</v>
+        <v>45908.250231481485</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>food</v>
+        <v>Travel</v>
       </c>
       <c r="B3">
-        <v>4000</v>
+        <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>45881.250231481485</v>
+        <v>45907.250231481485</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Tuition fee</v>
+        <v>Food</v>
       </c>
       <c r="B4">
-        <v>90000</v>
+        <v>2000</v>
       </c>
       <c r="C4" s="1">
-        <v>45873.250231481485</v>
+        <v>45906.250231481485</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Travel</v>
+        <v>Food</v>
       </c>
       <c r="B5">
-        <v>4000</v>
+        <v>1200</v>
       </c>
       <c r="C5" s="1">
-        <v>45872.250231481485</v>
+        <v>45905.250231481485</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>Games</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45904.250231481485</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Extra</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45903.250231481485</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
         <v>Food</v>
       </c>
-      <c r="B6">
+      <c r="B8">
+        <v>1500</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45903.250231481485</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>cat</v>
+      </c>
+      <c r="B9">
+        <v>30000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45883.250231481485</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Tuition fee</v>
+      </c>
+      <c r="B10">
+        <v>90000</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45873.250231481485</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Food</v>
+      </c>
+      <c r="B11">
         <v>10000</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C11" s="1">
         <v>45870.250231481485</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>